<commit_message>
Directory Adjustment and Excel Cells to Image
</commit_message>
<xml_diff>
--- a/Excel/List Tugas Gabunggan.xlsx
+++ b/Excel/List Tugas Gabunggan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\System Support\Tugas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev\Web Kelas\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A282777-7B86-40BF-AC29-F914D8E39546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FEC06C-E1DC-47A0-84CF-A4FACA5E6485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="125">
   <si>
     <t>No.</t>
   </si>
@@ -1137,7 +1137,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA15" sqref="AA15"/>
+      <selection pane="bottomRight" activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1733,7 +1733,9 @@
       <c r="S8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="16"/>
+      <c r="T8" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="U8" s="15" t="s">
         <v>12</v>
       </c>
@@ -1750,7 +1752,9 @@
         <v>12</v>
       </c>
       <c r="Z8" s="41"/>
-      <c r="AA8" s="44"/>
+      <c r="AA8" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
@@ -2056,7 +2060,9 @@
       <c r="Z12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AA12" s="44"/>
+      <c r="AA12" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
@@ -3144,7 +3150,9 @@
       <c r="Z26" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AA26" s="44"/>
+      <c r="AA26" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="27" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
@@ -3382,7 +3390,9 @@
       <c r="Z29" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="AA29" s="44"/>
+      <c r="AA29" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
@@ -3504,7 +3514,9 @@
       <c r="X31" s="42"/>
       <c r="Y31" s="43"/>
       <c r="Z31" s="41"/>
-      <c r="AA31" s="44"/>
+      <c r="AA31" s="37" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="32" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
@@ -4100,7 +4112,7 @@
     <row r="40" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24">
         <f>COUNTA(C4:AA38)</f>
-        <v>764</v>
+        <v>770</v>
       </c>
       <c r="B40" s="55" t="s">
         <v>59</v>
@@ -4192,11 +4204,11 @@
     <row r="42" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24">
         <f>100 * A40 / A41</f>
-        <v>87.314285714285717</v>
+        <v>88</v>
       </c>
       <c r="B42" s="25">
         <f>TRUNC(A42,1)</f>
-        <v>87.3</v>
+        <v>88</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="7">
@@ -4423,7 +4435,7 @@
       <c r="H48" s="29"/>
       <c r="I48" s="28">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>

</xml_diff>

<commit_message>
Directory Adjustment, Updating Made Easier and Fixed Merge Cell Issue
</commit_message>
<xml_diff>
--- a/Excel/List Tugas Gabunggan.xlsx
+++ b/Excel/List Tugas Gabunggan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev\Web Kelas\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\System Support\Tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FEC06C-E1DC-47A0-84CF-A4FACA5E6485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8F36BB-E6F4-4A62-B85C-78CE59C53221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="127">
   <si>
     <t>No.</t>
   </si>
@@ -403,6 +403,12 @@
   </si>
   <si>
     <t>PWPB4</t>
+  </si>
+  <si>
+    <t>BINDO2</t>
+  </si>
+  <si>
+    <t>BINDO3</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -603,57 +609,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -753,12 +713,6 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,28 +737,25 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,16 +764,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1131,109 +1079,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA98"/>
+  <dimension ref="A1:AC98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R42" sqref="R42"/>
+      <selection pane="bottomRight" activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="25" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="27" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:29" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="58" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="49" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="47" t="s">
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="45" t="s">
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="46"/>
-    </row>
-    <row r="2" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="35" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+    </row>
+    <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="36" t="s">
+      <c r="M2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="44" t="s">
         <v>49</v>
       </c>
       <c r="P2" s="3" t="s">
@@ -1272,10 +1222,16 @@
       <c r="AA2" s="33" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="AB2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="4" t="s">
         <v>60</v>
       </c>
@@ -1351,8 +1307,14 @@
       <c r="AA3" s="34" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB3" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC3" s="34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1420,23 +1382,25 @@
       <c r="V4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W4" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X4" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y4" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z4" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA4" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y4" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="39"/>
+      <c r="AC4" s="42"/>
+    </row>
+    <row r="5" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -1504,19 +1468,21 @@
       <c r="V5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X5" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y5" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="44"/>
-    </row>
-    <row r="6" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X5" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z5" s="39"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="39"/>
+      <c r="AC5" s="42"/>
+    </row>
+    <row r="6" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -1584,27 +1550,29 @@
       <c r="V6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W6" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X6" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y6" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X6" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y6" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="42"/>
+    </row>
+    <row r="7" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="str">
         <f>IF(I47 &lt;= P41, D47, B47)</f>
-        <v>Arif Fathurrahman</v>
+        <v>Arif Fathurrahman,</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>12</v>
@@ -1664,17 +1632,19 @@
       <c r="V7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W7" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X7" s="42"/>
-      <c r="Y7" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="44"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z7" s="39"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="39"/>
+      <c r="AC7" s="42"/>
+    </row>
+    <row r="8" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -1742,21 +1712,23 @@
       <c r="V8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W8" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X8" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W8" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="39"/>
+      <c r="AA8" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="42"/>
+    </row>
+    <row r="9" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -1818,17 +1790,19 @@
       <c r="T9" s="16"/>
       <c r="U9" s="13"/>
       <c r="V9" s="16"/>
-      <c r="W9" s="43"/>
-      <c r="X9" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="44"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W9" s="41"/>
+      <c r="X9" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y9" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z9" s="39"/>
+      <c r="AA9" s="42"/>
+      <c r="AB9" s="39"/>
+      <c r="AC9" s="42"/>
+    </row>
+    <row r="10" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -1896,19 +1870,21 @@
       <c r="V10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W10" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X10" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y10" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="44"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X10" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y10" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z10" s="39"/>
+      <c r="AA10" s="42"/>
+      <c r="AB10" s="39"/>
+      <c r="AC10" s="42"/>
+    </row>
+    <row r="11" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -1974,13 +1950,15 @@
         <v>12</v>
       </c>
       <c r="V11" s="16"/>
-      <c r="W11" s="43"/>
-      <c r="X11" s="42"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="44"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W11" s="41"/>
+      <c r="X11" s="40"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="39"/>
+      <c r="AA11" s="42"/>
+      <c r="AB11" s="39"/>
+      <c r="AC11" s="42"/>
+    </row>
+    <row r="12" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -2048,23 +2026,25 @@
       <c r="V12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W12" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X12" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y12" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z12" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA12" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA12" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB12" s="39"/>
+      <c r="AC12" s="42"/>
+    </row>
+    <row r="13" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -2126,17 +2106,19 @@
       </c>
       <c r="U13" s="13"/>
       <c r="V13" s="16"/>
-      <c r="W13" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X13" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y13" s="43"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="44"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W13" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X13" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="39"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="39"/>
+      <c r="AC13" s="42"/>
+    </row>
+    <row r="14" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -2204,19 +2186,21 @@
       <c r="V14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W14" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X14" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y14" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="44"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W14" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X14" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y14" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="42"/>
+      <c r="AB14" s="39"/>
+      <c r="AC14" s="42"/>
+    </row>
+    <row r="15" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -2284,21 +2268,23 @@
       <c r="V15" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W15" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X15" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y15" s="43" t="s">
+      <c r="W15" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X15" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y15" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB15" s="39"/>
+      <c r="AC15" s="42"/>
+    </row>
+    <row r="16" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -2366,25 +2352,27 @@
       <c r="V16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W16" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z16" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA16" s="44"/>
-    </row>
-    <row r="17" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W16" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="40"/>
+      <c r="Y16" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="42"/>
+      <c r="AB16" s="39"/>
+      <c r="AC16" s="42"/>
+    </row>
+    <row r="17" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>14</v>
       </c>
       <c r="B17" s="2" t="str">
         <f>IF(I57 &lt;= P41, D57, B57)</f>
-        <v>Muhammad Akbar Ariq Jeconia Lesmana</v>
+        <v>Muhammad Akbar Ariq Jeconia Lesmana,</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>12</v>
@@ -2442,19 +2430,21 @@
       <c r="V17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W17" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X17" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y17" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="44"/>
-    </row>
-    <row r="18" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W17" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X17" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y17" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z17" s="39"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="39"/>
+      <c r="AC17" s="42"/>
+    </row>
+    <row r="18" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>15</v>
       </c>
@@ -2520,25 +2510,27 @@
       <c r="V18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W18" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X18" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y18" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="44"/>
-    </row>
-    <row r="19" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W18" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X18" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y18" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z18" s="39"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="39"/>
+      <c r="AC18" s="42"/>
+    </row>
+    <row r="19" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="str">
         <f>IF(I59 &lt;= P41, D59, B59)</f>
-        <v>Muhammad Athala Romero</v>
+        <v>Muhammad Athala Romero,</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>12</v>
@@ -2594,23 +2586,25 @@
       <c r="V19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W19" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X19" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y19" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z19" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA19" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W19" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X19" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y19" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z19" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA19" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB19" s="39"/>
+      <c r="AC19" s="42"/>
+    </row>
+    <row r="20" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>17</v>
       </c>
@@ -2676,19 +2670,21 @@
       <c r="V20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W20" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X20" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y20" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="44"/>
-    </row>
-    <row r="21" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W20" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X20" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y20" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z20" s="39"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="39"/>
+      <c r="AC20" s="42"/>
+    </row>
+    <row r="21" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>18</v>
       </c>
@@ -2754,19 +2750,21 @@
       <c r="V21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X21" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y21" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="44"/>
-    </row>
-    <row r="22" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W21" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X21" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y21" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z21" s="39"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="39"/>
+      <c r="AC21" s="42"/>
+    </row>
+    <row r="22" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>19</v>
       </c>
@@ -2834,19 +2832,21 @@
       <c r="V22" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W22" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X22" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y22" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z22" s="41"/>
-      <c r="AA22" s="44"/>
-    </row>
-    <row r="23" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W22" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X22" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z22" s="39"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="39"/>
+      <c r="AC22" s="42"/>
+    </row>
+    <row r="23" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>20</v>
       </c>
@@ -2910,15 +2910,17 @@
         <v>12</v>
       </c>
       <c r="V23" s="16"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="42"/>
-      <c r="Y23" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z23" s="41"/>
-      <c r="AA23" s="44"/>
-    </row>
-    <row r="24" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W23" s="41"/>
+      <c r="X23" s="40"/>
+      <c r="Y23" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z23" s="39"/>
+      <c r="AA23" s="42"/>
+      <c r="AB23" s="39"/>
+      <c r="AC23" s="42"/>
+    </row>
+    <row r="24" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>21</v>
       </c>
@@ -2980,17 +2982,19 @@
       <c r="V24" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W24" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z24" s="41"/>
-      <c r="AA24" s="44"/>
-    </row>
-    <row r="25" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W24" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X24" s="40"/>
+      <c r="Y24" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z24" s="39"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="39"/>
+      <c r="AC24" s="42"/>
+    </row>
+    <row r="25" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>22</v>
       </c>
@@ -3058,19 +3062,21 @@
       <c r="V25" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W25" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X25" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y25" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z25" s="41"/>
-      <c r="AA25" s="44"/>
-    </row>
-    <row r="26" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W25" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X25" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y25" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z25" s="39"/>
+      <c r="AA25" s="42"/>
+      <c r="AB25" s="39"/>
+      <c r="AC25" s="42"/>
+    </row>
+    <row r="26" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>23</v>
       </c>
@@ -3138,23 +3144,25 @@
       <c r="V26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W26" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X26" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y26" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z26" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA26" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W26" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X26" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y26" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z26" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA26" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB26" s="39"/>
+      <c r="AC26" s="42"/>
+    </row>
+    <row r="27" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>24</v>
       </c>
@@ -3222,25 +3230,27 @@
       <c r="V27" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W27" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X27" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y27" s="43" t="s">
+      <c r="W27" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X27" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y27" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="Z27" s="41"/>
-      <c r="AA27" s="44"/>
-    </row>
-    <row r="28" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="42"/>
+      <c r="AB27" s="39"/>
+      <c r="AC27" s="42"/>
+    </row>
+    <row r="28" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>25</v>
       </c>
       <c r="B28" s="2" t="str">
         <f>IF(I68 &lt;= P41, D68, B68)</f>
-        <v>Nouridza Juniansah Ridhan</v>
+        <v>Nouridza Juniansah Ridhan,</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
@@ -3300,17 +3310,19 @@
       <c r="V28" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W28" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X28" s="42"/>
-      <c r="Y28" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="44"/>
-    </row>
-    <row r="29" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W28" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X28" s="40"/>
+      <c r="Y28" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="42"/>
+      <c r="AB28" s="39"/>
+      <c r="AC28" s="42"/>
+    </row>
+    <row r="29" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>26</v>
       </c>
@@ -3378,23 +3390,25 @@
       <c r="V29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W29" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X29" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y29" s="43" t="s">
+      <c r="W29" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X29" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y29" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="Z29" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA29" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Z29" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA29" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB29" s="39"/>
+      <c r="AC29" s="42"/>
+    </row>
+    <row r="30" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>27</v>
       </c>
@@ -3444,13 +3458,15 @@
       </c>
       <c r="U30" s="13"/>
       <c r="V30" s="16"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="44"/>
-    </row>
-    <row r="31" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W30" s="41"/>
+      <c r="X30" s="40"/>
+      <c r="Y30" s="41"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="42"/>
+      <c r="AB30" s="39"/>
+      <c r="AC30" s="42"/>
+    </row>
+    <row r="31" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>28</v>
       </c>
@@ -3508,17 +3524,19 @@
         <v>12</v>
       </c>
       <c r="V31" s="16"/>
-      <c r="W31" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="41"/>
-      <c r="AA31" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W31" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="39"/>
+      <c r="AA31" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB31" s="39"/>
+      <c r="AC31" s="42"/>
+    </row>
+    <row r="32" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>29</v>
       </c>
@@ -3586,29 +3604,31 @@
       <c r="V32" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W32" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X32" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y32" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z32" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA32" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W32" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X32" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y32" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z32" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA32" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB32" s="39"/>
+      <c r="AC32" s="42"/>
+    </row>
+    <row r="33" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>30</v>
       </c>
       <c r="B33" s="2" t="str">
         <f>IF(I73 &lt;= P41, D73, B73)</f>
-        <v>Salsabila Nur Fairuz</v>
+        <v>Salsabila Nur Fairuz,</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>12</v>
@@ -3668,17 +3688,21 @@
       <c r="V33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W33" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X33" s="39"/>
-      <c r="Y33" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z33" s="41"/>
-      <c r="AA33" s="44"/>
-    </row>
-    <row r="34" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W33" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X33" s="37"/>
+      <c r="Y33" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z33" s="39"/>
+      <c r="AA33" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB33" s="39"/>
+      <c r="AC33" s="42"/>
+    </row>
+    <row r="34" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>31</v>
       </c>
@@ -3746,19 +3770,25 @@
       <c r="V34" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W34" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X34" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y34" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z34" s="41"/>
-      <c r="AA34" s="44"/>
-    </row>
-    <row r="35" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W34" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X34" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y34" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z34" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA34" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB34" s="39"/>
+      <c r="AC34" s="42"/>
+    </row>
+    <row r="35" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>32</v>
       </c>
@@ -3826,21 +3856,23 @@
       <c r="V35" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W35" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X35" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y35" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z35" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA35" s="44"/>
-    </row>
-    <row r="36" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W35" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X35" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y35" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z35" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA35" s="42"/>
+      <c r="AB35" s="39"/>
+      <c r="AC35" s="42"/>
+    </row>
+    <row r="36" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>33</v>
       </c>
@@ -3908,23 +3940,25 @@
       <c r="V36" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W36" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X36" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y36" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z36" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA36" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W36" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X36" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y36" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z36" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA36" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB36" s="39"/>
+      <c r="AC36" s="42"/>
+    </row>
+    <row r="37" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>34</v>
       </c>
@@ -3992,25 +4026,27 @@
       <c r="V37" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="W37" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X37" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y37" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z37" s="41"/>
-      <c r="AA37" s="44"/>
-    </row>
-    <row r="38" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="W37" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X37" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y37" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z37" s="39"/>
+      <c r="AA37" s="42"/>
+      <c r="AB37" s="39"/>
+      <c r="AC37" s="42"/>
+    </row>
+    <row r="38" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>35</v>
       </c>
       <c r="B38" s="2" t="str">
         <f>IF(I78 &lt;= P41, D78, B78)</f>
-        <v>Yehezkiel Dio Sinolungan</v>
+        <v>Yehezkiel Dio Sinolungan,</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>12</v>
@@ -4068,21 +4104,23 @@
         <v>12</v>
       </c>
       <c r="V38" s="16"/>
-      <c r="W38" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="X38" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y38" s="43" t="s">
+      <c r="W38" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="X38" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y38" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="Z38" s="41"/>
-      <c r="AA38" s="37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="Z38" s="39"/>
+      <c r="AA38" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB38" s="39"/>
+      <c r="AC38" s="42"/>
+    </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -4109,34 +4147,34 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
     </row>
-    <row r="40" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24">
-        <f>COUNTA(C4:AA38)</f>
-        <v>770</v>
-      </c>
-      <c r="B40" s="55" t="s">
+        <f>COUNTA(C4:AC38)</f>
+        <v>773</v>
+      </c>
+      <c r="B40" s="45" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="52"/>
-      <c r="F40" s="52"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="52"/>
-      <c r="K40" s="52"/>
-      <c r="L40" s="52"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="53" t="s">
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="50" t="s">
         <v>80</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="26">
-        <f>COUNTA(C3:AA3)</f>
-        <v>25</v>
+        <f>COUNTA(C3:AC3)</f>
+        <v>27</v>
       </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
@@ -4148,12 +4186,12 @@
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
     </row>
-    <row r="41" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24">
         <f>P40 * 35</f>
-        <v>875</v>
-      </c>
-      <c r="B41" s="56"/>
+        <v>945</v>
+      </c>
+      <c r="B41" s="46"/>
       <c r="C41" s="1"/>
       <c r="D41" s="32" t="s">
         <v>7</v>
@@ -4185,11 +4223,11 @@
       <c r="M41" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="N41" s="54"/>
+      <c r="N41" s="51"/>
       <c r="O41" s="1"/>
       <c r="P41" s="26">
         <f>P40-6</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
@@ -4201,14 +4239,14 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
     </row>
-    <row r="42" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24">
         <f>100 * A40 / A41</f>
-        <v>88</v>
+        <v>81.798941798941797</v>
       </c>
       <c r="B42" s="25">
         <f>TRUNC(A42,1)</f>
-        <v>88</v>
+        <v>81.7</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="7">
@@ -4230,7 +4268,7 @@
         <v>4</v>
       </c>
       <c r="J42" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K42" s="7">
         <v>1</v>
@@ -4243,7 +4281,7 @@
       </c>
       <c r="N42" s="7">
         <f>SUM(D42:M42)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
@@ -4257,7 +4295,7 @@
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
     </row>
-    <row r="43" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -4284,7 +4322,7 @@
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
     </row>
-    <row r="44" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="27" t="s">
         <v>11</v>
@@ -4318,7 +4356,7 @@
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
     </row>
-    <row r="45" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="27" t="s">
         <v>13</v>
@@ -4352,7 +4390,7 @@
       <c r="X45" s="1"/>
       <c r="Y45" s="1"/>
     </row>
-    <row r="46" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="27" t="s">
         <v>14</v>
@@ -4386,7 +4424,7 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
     </row>
-    <row r="47" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="27" t="s">
         <v>15</v>
@@ -4420,7 +4458,7 @@
       <c r="X47" s="1"/>
       <c r="Y47" s="1"/>
     </row>
-    <row r="48" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="27" t="s">
         <v>16</v>
@@ -5972,16 +6010,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="D40:M40"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="B40:B41"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="H1:O1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="P1:V1"/>
-    <mergeCell ref="D40:M40"/>
-    <mergeCell ref="N40:N41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>

<commit_message>
Combined Task to Image and Github Abous Us
</commit_message>
<xml_diff>
--- a/Excel/List Tugas Gabunggan.xlsx
+++ b/Excel/List Tugas Gabunggan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\System Support\Tugas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\Web Dev\Web Kelas\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8F36BB-E6F4-4A62-B85C-78CE59C53221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88DFA51-6A69-472B-8845-17F0F3DBAECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -743,19 +743,13 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,10 +761,16 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1082,10 +1082,10 @@
   <dimension ref="A1:AC98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB25" sqref="AB25"/>
+      <selection pane="bottomRight" activeCell="AC42" sqref="AC42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1106,43 +1106,43 @@
       <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="53" t="s">
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="54" t="s">
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="52" t="s">
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
     </row>
     <row r="2" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>
@@ -4152,7 +4152,7 @@
         <f>COUNTA(C4:AC38)</f>
         <v>773</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="51" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="1"/>
@@ -4168,7 +4168,7 @@
       <c r="K40" s="47"/>
       <c r="L40" s="47"/>
       <c r="M40" s="47"/>
-      <c r="N40" s="50" t="s">
+      <c r="N40" s="48" t="s">
         <v>80</v>
       </c>
       <c r="O40" s="1"/>
@@ -4191,7 +4191,7 @@
         <f>P40 * 35</f>
         <v>945</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="52"/>
       <c r="C41" s="1"/>
       <c r="D41" s="32" t="s">
         <v>7</v>
@@ -4223,7 +4223,7 @@
       <c r="M41" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="N41" s="51"/>
+      <c r="N41" s="49"/>
       <c r="O41" s="1"/>
       <c r="P41" s="26">
         <f>P40-6</f>
@@ -6010,16 +6010,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:O1"/>
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="D40:M40"/>
     <mergeCell ref="N40:N41"/>
     <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:O1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>

<commit_message>
Cursor Set To Default At Main Image Container & File Update
</commit_message>
<xml_diff>
--- a/Excel/List Tugas Gabunggan.xlsx
+++ b/Excel/List Tugas Gabunggan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\System Support\Tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7787E466-CFDF-4ABC-A980-9A597073A368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271E8F3E-D4B7-4608-89C7-B23101E54D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,6 +543,20 @@
       <sz val="14"/>
       <name val="Wingdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -698,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -822,33 +836,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -876,11 +863,39 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1191,10 +1206,10 @@
   <dimension ref="A1:AV78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BA22" sqref="BA22"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B44:B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1227,80 +1242,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49" t="s">
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="62" t="s">
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="61" t="s">
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="48" t="s">
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="49" t="s">
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="55"/>
+      <c r="AG1" s="55"/>
+      <c r="AH1" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="59" t="s">
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="60"/>
-      <c r="AP1" s="57" t="s">
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="AQ1" s="58"/>
-      <c r="AR1" s="58"/>
-      <c r="AS1" s="58"/>
-      <c r="AT1" s="58"/>
-      <c r="AU1" s="52" t="s">
+      <c r="AQ1" s="49"/>
+      <c r="AR1" s="49"/>
+      <c r="AS1" s="49"/>
+      <c r="AT1" s="49"/>
+      <c r="AU1" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="AV1" s="53"/>
+      <c r="AV1" s="44"/>
     </row>
     <row r="2" spans="1:48" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
@@ -1441,8 +1456,8 @@
       </c>
     </row>
     <row r="3" spans="1:48" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="30" t="s">
         <v>59</v>
       </c>
@@ -6244,26 +6259,26 @@
         <f>COUNTA(C4:AV38)</f>
         <v>1366</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="54" t="s">
+      <c r="D40" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="55"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="55"/>
-      <c r="N40" s="56"/>
-      <c r="O40" s="50" t="s">
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="Q40" s="2">
+      <c r="Q40" s="61">
         <f>COUNTA(C3:AV3)</f>
         <v>46</v>
       </c>
@@ -6273,7 +6288,7 @@
         <f>Q40 * 35</f>
         <v>1610</v>
       </c>
-      <c r="B41" s="46"/>
+      <c r="B41" s="57"/>
       <c r="D41" s="39" t="s">
         <v>7</v>
       </c>
@@ -6307,8 +6322,8 @@
       <c r="N41" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="O41" s="51"/>
-      <c r="Q41" s="2">
+      <c r="O41" s="60"/>
+      <c r="Q41" s="61">
         <f>Q40-6</f>
         <v>40</v>
       </c>
@@ -6362,602 +6377,608 @@
     </row>
     <row r="43" spans="1:48" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="63" t="s">
         <v>11</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="43" t="s">
+      <c r="D44" s="63" t="s">
         <v>83</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="44">
+      <c r="I44" s="62">
         <f>COUNTA(C4:AV4)</f>
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="63" t="s">
         <v>13</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" s="43" t="s">
+      <c r="D45" s="63" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="44">
+      <c r="I45" s="62">
         <f t="shared" ref="I45:I78" si="0">COUNTA(C5:AV5)</f>
         <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:48" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="43" t="s">
+      <c r="B46" s="63" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="43" t="s">
+      <c r="D46" s="63" t="s">
         <v>85</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="44">
+      <c r="I46" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:48" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="63" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="5"/>
-      <c r="D47" s="43" t="s">
+      <c r="D47" s="63" t="s">
         <v>86</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="44">
+      <c r="I47" s="62">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:48" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="43" t="s">
+      <c r="B48" s="63" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="5"/>
-      <c r="D48" s="43" t="s">
+      <c r="D48" s="63" t="s">
         <v>87</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="44">
+      <c r="I48" s="62">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="43" t="s">
+      <c r="B49" s="63" t="s">
         <v>17</v>
       </c>
       <c r="C49" s="5"/>
-      <c r="D49" s="43" t="s">
+      <c r="D49" s="63" t="s">
         <v>88</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="44">
+      <c r="I49" s="62">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="43" t="s">
+      <c r="B50" s="63" t="s">
         <v>18</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="43" t="s">
+      <c r="D50" s="63" t="s">
         <v>89</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
-      <c r="I50" s="44">
+      <c r="I50" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="43" t="s">
+      <c r="B51" s="63" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="5"/>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="63" t="s">
         <v>90</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
-      <c r="I51" s="44">
+      <c r="I51" s="62">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="52" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="63" t="s">
         <v>20</v>
       </c>
       <c r="C52" s="5"/>
-      <c r="D52" s="43" t="s">
+      <c r="D52" s="63" t="s">
         <v>91</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
-      <c r="I52" s="44">
+      <c r="I52" s="62">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B53" s="43" t="s">
+      <c r="B53" s="63" t="s">
         <v>21</v>
       </c>
       <c r="C53" s="5"/>
-      <c r="D53" s="43" t="s">
+      <c r="D53" s="63" t="s">
         <v>92</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
-      <c r="I53" s="44">
+      <c r="I53" s="62">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
     <row r="54" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="43" t="s">
+      <c r="B54" s="63" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="5"/>
-      <c r="D54" s="43" t="s">
+      <c r="D54" s="63" t="s">
         <v>93</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-      <c r="I54" s="44">
+      <c r="I54" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="63" t="s">
         <v>23</v>
       </c>
       <c r="C55" s="5"/>
-      <c r="D55" s="43" t="s">
+      <c r="D55" s="63" t="s">
         <v>94</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-      <c r="I55" s="44">
+      <c r="I55" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B56" s="43" t="s">
+      <c r="B56" s="63" t="s">
         <v>24</v>
       </c>
       <c r="C56" s="5"/>
-      <c r="D56" s="43" t="s">
+      <c r="D56" s="63" t="s">
         <v>95</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="44">
+      <c r="I56" s="62">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="63" t="s">
         <v>25</v>
       </c>
       <c r="C57" s="5"/>
-      <c r="D57" s="43" t="s">
+      <c r="D57" s="63" t="s">
         <v>96</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="44">
+      <c r="I57" s="62">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B58" s="43" t="s">
+      <c r="B58" s="63" t="s">
         <v>26</v>
       </c>
       <c r="C58" s="5"/>
-      <c r="D58" s="43" t="s">
+      <c r="D58" s="63" t="s">
         <v>97</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="44">
+      <c r="I58" s="62">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B59" s="43" t="s">
+      <c r="B59" s="63" t="s">
         <v>27</v>
       </c>
       <c r="C59" s="5"/>
-      <c r="D59" s="43" t="s">
+      <c r="D59" s="63" t="s">
         <v>98</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
-      <c r="I59" s="44">
+      <c r="I59" s="62">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="63" t="s">
         <v>28</v>
       </c>
       <c r="C60" s="5"/>
-      <c r="D60" s="43" t="s">
+      <c r="D60" s="63" t="s">
         <v>99</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="44">
+      <c r="I60" s="62">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="61" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="63" t="s">
         <v>29</v>
       </c>
       <c r="C61" s="5"/>
-      <c r="D61" s="43" t="s">
+      <c r="D61" s="63" t="s">
         <v>100</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="44">
+      <c r="I61" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B62" s="43" t="s">
+      <c r="B62" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C62" s="5"/>
-      <c r="D62" s="43" t="s">
+      <c r="D62" s="63" t="s">
         <v>101</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-      <c r="I62" s="44">
+      <c r="I62" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="63" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="43" t="s">
+      <c r="B63" s="63" t="s">
         <v>31</v>
       </c>
       <c r="C63" s="5"/>
-      <c r="D63" s="43" t="s">
+      <c r="D63" s="63" t="s">
         <v>102</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="44">
+      <c r="I63" s="62">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B64" s="43" t="s">
+      <c r="B64" s="63" t="s">
         <v>32</v>
       </c>
       <c r="C64" s="5"/>
-      <c r="D64" s="43" t="s">
+      <c r="D64" s="63" t="s">
         <v>82</v>
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-      <c r="I64" s="44">
+      <c r="I64" s="62">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="63" t="s">
         <v>33</v>
       </c>
       <c r="C65" s="5"/>
-      <c r="D65" s="43" t="s">
+      <c r="D65" s="63" t="s">
         <v>116</v>
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65" s="44">
+      <c r="I65" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="66" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="43" t="s">
+      <c r="B66" s="63" t="s">
         <v>34</v>
       </c>
       <c r="C66" s="5"/>
-      <c r="D66" s="43" t="s">
+      <c r="D66" s="63" t="s">
         <v>103</v>
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
-      <c r="I66" s="44">
+      <c r="I66" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="63" t="s">
         <v>35</v>
       </c>
       <c r="C67" s="5"/>
-      <c r="D67" s="43" t="s">
+      <c r="D67" s="63" t="s">
         <v>104</v>
       </c>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
-      <c r="I67" s="44">
+      <c r="I67" s="62">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="68" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B68" s="43" t="s">
+      <c r="B68" s="63" t="s">
         <v>36</v>
       </c>
       <c r="C68" s="5"/>
-      <c r="D68" s="43" t="s">
+      <c r="D68" s="63" t="s">
         <v>105</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
-      <c r="I68" s="44">
+      <c r="I68" s="62">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="69" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="63" t="s">
         <v>37</v>
       </c>
       <c r="C69" s="5"/>
-      <c r="D69" s="43" t="s">
+      <c r="D69" s="63" t="s">
         <v>106</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
-      <c r="I69" s="44">
+      <c r="I69" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="70" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="63" t="s">
         <v>38</v>
       </c>
       <c r="C70" s="5"/>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="63" t="s">
         <v>107</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
-      <c r="I70" s="44">
+      <c r="I70" s="62">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
     <row r="71" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B71" s="43" t="s">
+      <c r="B71" s="63" t="s">
         <v>39</v>
       </c>
       <c r="C71" s="5"/>
-      <c r="D71" s="43" t="s">
+      <c r="D71" s="63" t="s">
         <v>108</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
-      <c r="I71" s="44">
+      <c r="I71" s="62">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="72" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="63" t="s">
         <v>40</v>
       </c>
       <c r="C72" s="5"/>
-      <c r="D72" s="43" t="s">
+      <c r="D72" s="63" t="s">
         <v>109</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
-      <c r="I72" s="44">
+      <c r="I72" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="73" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B73" s="43" t="s">
+      <c r="B73" s="63" t="s">
         <v>41</v>
       </c>
       <c r="C73" s="5"/>
-      <c r="D73" s="43" t="s">
+      <c r="D73" s="63" t="s">
         <v>110</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
       <c r="H73" s="5"/>
-      <c r="I73" s="44">
+      <c r="I73" s="62">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="74" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B74" s="43" t="s">
+      <c r="B74" s="63" t="s">
         <v>42</v>
       </c>
       <c r="C74" s="5"/>
-      <c r="D74" s="43" t="s">
+      <c r="D74" s="63" t="s">
         <v>111</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
-      <c r="I74" s="44">
+      <c r="I74" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="75" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B75" s="43" t="s">
+      <c r="B75" s="63" t="s">
         <v>43</v>
       </c>
       <c r="C75" s="5"/>
-      <c r="D75" s="43" t="s">
+      <c r="D75" s="63" t="s">
         <v>112</v>
       </c>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
-      <c r="I75" s="44">
+      <c r="I75" s="62">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="76" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B76" s="43" t="s">
+      <c r="B76" s="63" t="s">
         <v>44</v>
       </c>
       <c r="C76" s="5"/>
-      <c r="D76" s="43" t="s">
+      <c r="D76" s="63" t="s">
         <v>113</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="44">
+      <c r="I76" s="62">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="77" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B77" s="43" t="s">
+      <c r="B77" s="63" t="s">
         <v>45</v>
       </c>
       <c r="C77" s="5"/>
-      <c r="D77" s="43" t="s">
+      <c r="D77" s="63" t="s">
         <v>115</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
-      <c r="I77" s="44">
+      <c r="I77" s="62">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
     <row r="78" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B78" s="43" t="s">
+      <c r="B78" s="63" t="s">
         <v>46</v>
       </c>
       <c r="C78" s="5"/>
-      <c r="D78" s="43" t="s">
+      <c r="D78" s="63" t="s">
         <v>114</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
-      <c r="I78" s="44">
+      <c r="I78" s="62">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:O1"/>
+    <mergeCell ref="O40:O41"/>
     <mergeCell ref="AU1:AV1"/>
     <mergeCell ref="D40:N40"/>
     <mergeCell ref="AP1:AT1"/>
@@ -6966,12 +6987,6 @@
     <mergeCell ref="W1:Y1"/>
     <mergeCell ref="P1:V1"/>
     <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="H1:O1"/>
-    <mergeCell ref="O40:O41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:B38">

</xml_diff>